<commit_message>
SL Modifica excel dettaglio consulenze
</commit_message>
<xml_diff>
--- a/inputs/support_fin.xlsx
+++ b/inputs/support_fin.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUP\Documents\GitHub\22p11_Tool_FA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5AE809B4-407A-4E48-B1A2-293026636153}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A831254-8A94-4C5F-8835-251C71FF7B59}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{3A038FE8-7C83-4276-93B2-F548EE42F943}"/>
   </bookViews>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="72">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="73">
   <si>
     <t>RAMO</t>
   </si>
@@ -256,6 +256,9 @@
   </si>
   <si>
     <t>cerved</t>
+  </si>
+  <si>
+    <t>scadenza</t>
   </si>
 </sst>
 </file>
@@ -351,7 +354,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="7">
     <border>
       <left/>
       <right/>
@@ -420,6 +423,15 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -432,7 +444,7 @@
     <xf numFmtId="166" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="71">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="43" fontId="2" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
@@ -614,6 +626,8 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="6" xfId="2" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
     <cellStyle name="Migliaia 3" xfId="4" xr:uid="{FF415F09-35CA-4948-8459-B1C1CC39DF80}"/>
@@ -1365,10 +1379,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2EE3E1A8-BCC1-4333-8367-C35E078672EE}">
-  <dimension ref="A1:C7"/>
+  <dimension ref="A1:D7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1382,7 +1396,7 @@
     <col min="15" max="15" width="11" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>71</v>
       </c>
@@ -1392,8 +1406,11 @@
       <c r="C1" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D1" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>60</v>
       </c>
@@ -1403,8 +1420,11 @@
       <c r="C2">
         <v>24000</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D2" s="71">
+        <v>44712</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>62</v>
       </c>
@@ -1414,8 +1434,11 @@
       <c r="C3">
         <v>10230</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D3" s="71">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>62</v>
       </c>
@@ -1425,8 +1448,11 @@
       <c r="C4">
         <v>20770</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D4" s="71">
+        <v>44681</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>64</v>
       </c>
@@ -1436,8 +1462,11 @@
       <c r="C5">
         <v>5000</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D5" s="71">
+        <v>44620</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>66</v>
       </c>
@@ -1447,8 +1476,11 @@
       <c r="C6">
         <v>35550</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="D6" s="71">
+        <v>44834</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>68</v>
       </c>
@@ -1457,6 +1489,9 @@
       </c>
       <c r="C7">
         <v>8250</v>
+      </c>
+      <c r="D7" s="72">
+        <v>44834</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
SL modifiche excel supporto fin
</commit_message>
<xml_diff>
--- a/inputs/support_fin.xlsx
+++ b/inputs/support_fin.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LUP\Documents\GitHub\22p11_Tool_FA\inputs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8AFDBB3-5757-47FD-9169-07EB38AF1B65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1C657FB-7693-4663-A6E3-2B85392CA46D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="3" xr2:uid="{3A038FE8-7C83-4276-93B2-F548EE42F943}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="5" xr2:uid="{3A038FE8-7C83-4276-93B2-F548EE42F943}"/>
   </bookViews>
   <sheets>
     <sheet name="Ipotesi" sheetId="6" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="59">
   <si>
     <t>RAMO</t>
   </si>
@@ -148,9 +148,6 @@
   </si>
   <si>
     <t>Incasso credito FMG</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Scadenza  </t>
   </si>
   <si>
     <t>Quota Capitale  </t>
@@ -228,8 +225,8 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
-    <numFmt numFmtId="166" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
-    <numFmt numFmtId="167" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
+    <numFmt numFmtId="164" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* \-??_-;_-@_-"/>
+    <numFmt numFmtId="165" formatCode="_-* #,##0.00\ [$€-410]_-;\-* #,##0.00\ [$€-410]_-;_-* &quot;-&quot;??\ [$€-410]_-;_-@_-"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -351,7 +348,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="27">
@@ -400,16 +397,16 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="6" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="2" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="14" fontId="4" fillId="4" borderId="2" xfId="6" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="2" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="2" xfId="7" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="167" fontId="4" fillId="4" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="165" fontId="4" fillId="4" borderId="2" xfId="7" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -752,13 +749,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -1186,24 +1183,24 @@
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C1" t="s">
+        <v>44</v>
+      </c>
+      <c r="D1" t="s">
         <v>57</v>
-      </c>
-      <c r="B1" t="s">
-        <v>56</v>
-      </c>
-      <c r="C1" t="s">
-        <v>45</v>
-      </c>
-      <c r="D1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B2" t="s">
         <v>46</v>
-      </c>
-      <c r="B2" t="s">
-        <v>47</v>
       </c>
       <c r="C2">
         <v>24000</v>
@@ -1214,10 +1211,10 @@
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
         <v>48</v>
-      </c>
-      <c r="B3" t="s">
-        <v>49</v>
       </c>
       <c r="C3">
         <v>10230</v>
@@ -1228,10 +1225,10 @@
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" t="s">
         <v>48</v>
-      </c>
-      <c r="B4" t="s">
-        <v>49</v>
       </c>
       <c r="C4">
         <v>20770</v>
@@ -1242,10 +1239,10 @@
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
         <v>50</v>
-      </c>
-      <c r="B5" t="s">
-        <v>51</v>
       </c>
       <c r="C5">
         <v>5000</v>
@@ -1256,10 +1253,10 @@
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
+        <v>51</v>
+      </c>
+      <c r="B6" t="s">
         <v>52</v>
-      </c>
-      <c r="B6" t="s">
-        <v>53</v>
       </c>
       <c r="C6">
         <v>35550</v>
@@ -1270,10 +1267,10 @@
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" t="s">
         <v>54</v>
-      </c>
-      <c r="B7" t="s">
-        <v>55</v>
       </c>
       <c r="C7">
         <v>8250</v>
@@ -1291,7 +1288,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E538E432-E0B4-4035-8EAC-19511E58C530}">
   <dimension ref="A1:F22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
+    <sheetView zoomScale="102" zoomScaleNormal="102" workbookViewId="0">
       <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
@@ -1307,22 +1304,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -1746,9 +1743,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1CF3E27B-4292-4F9B-970F-C016A4066077}">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -1762,22 +1757,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="8" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="8" t="s">
+      <c r="C1" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="8" t="s">
+      <c r="D1" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="8" t="s">
+      <c r="E1" s="8" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="8" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -2065,9 +2060,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{475E5D64-5758-4D31-9A94-64BD068F9A7A}">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
@@ -2081,22 +2074,22 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="17" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="17" t="s">
         <v>36</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="C1" s="17" t="s">
         <v>37</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="D1" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="E1" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="E1" s="17" t="s">
+      <c r="F1" s="17" t="s">
         <v>40</v>
-      </c>
-      <c r="F1" s="17" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>